<commit_message>
Updating and combining indoor cleaning
</commit_message>
<xml_diff>
--- a/data-original/08.07.22 ICS Seasonal Spreadsheet.xlsx
+++ b/data-original/08.07.22 ICS Seasonal Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilydemotte/MIG/tdcj-prison-heat/data-original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B87A0B-D3A9-F44A-A25F-2BFEAF703B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FB400C-2D58-8C4A-8572-7FC59C700580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="3040" windowWidth="16240" windowHeight="9340" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5540" yWindow="500" windowWidth="23260" windowHeight="11880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit &amp; County" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <author>tc={FB9DC052-091B-4A3A-9206-CAB85FAF745E}</author>
     <author>tc={E8967BBD-B500-40F0-AB5F-E28BDA860232}</author>
     <author>tc={392F9A56-5432-42DE-9E74-96C12BA60F9C}</author>
+    <author>Emily DeMotte</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0" shapeId="0" xr:uid="{B00FDFFB-3CBE-4203-99C4-723AEC06FA2F}">
@@ -227,6 +228,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="E29" authorId="7" shapeId="0" xr:uid="{D5302CC8-B26B-9840-AEC6-8A13D7F53827}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Emily DeMotte:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Corrected from 12/21/01 to 07/21/22</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -731,7 +765,7 @@
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -759,6 +793,19 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2434,8 +2481,8 @@
   </sheetPr>
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3176,7 +3223,7 @@
         <v>70</v>
       </c>
       <c r="E29" s="25">
-        <v>721</v>
+        <v>44763</v>
       </c>
       <c r="F29" s="18">
         <v>0.66666666666666663</v>

</xml_diff>